<commit_message>
Correction : support fichiers .xls et mise à jour requirements
</commit_message>
<xml_diff>
--- a/Livraison_finale_avec_ville_et_client.xlsx
+++ b/Livraison_finale_avec_ville_et_client.xlsx
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>60.14</v>
+        <v>120.28</v>
       </c>
       <c r="F2" t="n">
         <v>0.11201032</v>
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>98.28</v>
+        <v>294.84</v>
       </c>
       <c r="F3" t="n">
         <v>0.505174</v>
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>40.08</v>
+        <v>80.16</v>
       </c>
       <c r="F4" t="n">
         <v>0.3576669</v>
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>134.42</v>
+        <v>1747.46</v>
       </c>
       <c r="F5" t="n">
         <v>1.39778068</v>
@@ -651,14 +651,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>6012A10-1, 6012A10-1, 6012A10-1, 6012A10-1, 1929A18-1, 1929A18-1, 1918A10-1, 1911A10-1, 1973C00-1, 1972A00-1, 1917A10-1, 1929A18-1, 1929A18-1, 1932A10-1, 6001A10-1</t>
+          <t>6012A10-1, 6012A10-1, 1929A18-1, 1918A10-1, 1911A10-1, 1973C00-1, 1972A00-1, 1917A10-1, 1929A18-1, 1932A10-1, 6001A10-1</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>77.03</v>
+        <v>669.13</v>
       </c>
       <c r="F8" t="n">
-        <v>0.56248551</v>
+        <v>0.43090675</v>
       </c>
     </row>
     <row r="9">
@@ -683,7 +683,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>28.935</v>
+        <v>115.74</v>
       </c>
       <c r="F9" t="n">
         <v>0.3933</v>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>5.895</v>
+        <v>11.79</v>
       </c>
       <c r="F10" t="n">
         <v>0.05264</v>
@@ -739,7 +739,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>30.245</v>
+        <v>90.73499999999999</v>
       </c>
       <c r="F11" t="n">
         <v>0.24287844</v>
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>163.16</v>
+        <v>1305.28</v>
       </c>
       <c r="F12" t="n">
         <v>1.97044348</v>
@@ -791,14 +791,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>6001A10-1, 6001A10-1, 6001A10-1, 6001A10-1</t>
+          <t>6001A10-1, 6001A10-1</t>
         </is>
       </c>
       <c r="E13" t="n">
         <v>140</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2242</v>
+        <v>0.1121</v>
       </c>
     </row>
     <row r="14">
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>158.12</v>
+        <v>316.24</v>
       </c>
       <c r="F14" t="n">
         <v>1.56423237</v>
@@ -851,7 +851,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>47.546</v>
+        <v>190.184</v>
       </c>
       <c r="F15" t="n">
         <v>0.23289354</v>
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>8.68</v>
+        <v>17.36</v>
       </c>
       <c r="F16" t="n">
         <v>0.04336677</v>
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>8.600000000000001</v>
+        <v>17.2</v>
       </c>
       <c r="F17" t="n">
         <v>0.07949753</v>
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>22.2</v>
+        <v>44.4</v>
       </c>
       <c r="F18" t="n">
         <v>0.2881762</v>
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>1.42</v>
+        <v>2.84</v>
       </c>
       <c r="F20" t="n">
         <v>0.0102635</v>
@@ -1015,14 +1015,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>SB75A04-1, SB75A04-1, SB57A04-1, SB75A04-1, SB75A04-1, SB65A04-1</t>
+          <t>SB75A04-1, SB57A04-1, SB75A04-1, SB65A04-1</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>5.501</v>
+        <v>13.184</v>
       </c>
       <c r="F21" t="n">
-        <v>0.02871405</v>
+        <v>0.01817235</v>
       </c>
     </row>
     <row r="22">
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>4.318</v>
+        <v>12.954</v>
       </c>
       <c r="F22" t="n">
         <v>0.025442025</v>
@@ -1071,14 +1071,14 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>SB82A04-1, SB82A04-1, SB57A04-1, SB57A04-1, SB57A04-1, SB57A04-1, SB82A04-1, SB82A04-1</t>
+          <t>SB82A04-1, SB57A04-1, SB57A04-1, SB82A04-1</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>14.862</v>
+        <v>29.724</v>
       </c>
       <c r="F23" t="n">
-        <v>0.07732800000000001</v>
+        <v>0.038664</v>
       </c>
     </row>
     <row r="24">
@@ -1099,14 +1099,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>SB51A04-1, SB51A04-1, SB82A04-1, SB82A04-1, SB57A04-1, SB82A04-1, SB82A04-1, SB51A04-1, SB51A04-1</t>
+          <t>SB51A04-1, SB82A04-1, SB57A04-1, SB82A04-1, SB51A04-1</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>27.7</v>
+        <v>88.75</v>
       </c>
       <c r="F24" t="n">
-        <v>0.182016</v>
+        <v>0.119088</v>
       </c>
     </row>
     <row r="25">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>6.487</v>
+        <v>12.974</v>
       </c>
       <c r="F25" t="n">
         <v>0.033588</v>
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>12.05</v>
+        <v>24.1</v>
       </c>
       <c r="F26" t="n">
         <v>0.08892</v>
@@ -1187,7 +1187,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>36.628</v>
+        <v>109.884</v>
       </c>
       <c r="F27" t="n">
         <v>0.240156</v>
@@ -1211,14 +1211,14 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>SB62A04-1, SB51A04-1, SB49A04-1, SB50A04-1, SB27A04-1, SB27A04-1, SB27A04-1, SB27A04-1, SB37A04-1</t>
+          <t>SB62A04-1, SB51A04-1, SB49A04-1, SB50A04-1, SB27A04-1, SB27A04-1, SB37A04-1</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>38.8</v>
+        <v>208.88</v>
       </c>
       <c r="F28" t="n">
-        <v>0.300003185</v>
+        <v>0.234938185</v>
       </c>
     </row>
     <row r="29">
@@ -1243,7 +1243,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>9.942</v>
+        <v>39.768</v>
       </c>
       <c r="F29" t="n">
         <v>0.06481774999999999</v>
@@ -1299,7 +1299,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>65.48999999999999</v>
+        <v>851.3699999999999</v>
       </c>
       <c r="F31" t="n">
         <v>0.53023367</v>
@@ -1327,7 +1327,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>13.94</v>
+        <v>27.88</v>
       </c>
       <c r="F32" t="n">
         <v>0.09809079999999999</v>
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>7.6</v>
+        <v>15.2</v>
       </c>
       <c r="F33" t="n">
         <v>0.0331872</v>
@@ -1411,7 +1411,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>3.816</v>
+        <v>7.632</v>
       </c>
       <c r="F35" t="n">
         <v>0.015768</v>
@@ -1463,14 +1463,14 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>04DBA04-1, 06DHA04-1, 06DHA04-1, 06DHA04-1, 06DHA04-1, 06DJA04-1</t>
+          <t>04DBA04-1, 06DHA04-1, 06DHA04-1, 06DJA04-1</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>12.59</v>
+        <v>35.48</v>
       </c>
       <c r="F37" t="n">
-        <v>0.04096604</v>
+        <v>0.02962604</v>
       </c>
     </row>
     <row r="38">
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>402.185</v>
+        <v>2010.925</v>
       </c>
       <c r="F38" t="n">
         <v>0.85839345</v>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1559.2</v>
+        <v>21828.8</v>
       </c>
       <c r="F39" t="n">
         <v>1.3604166</v>
@@ -1551,7 +1551,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>1529</v>
+        <v>19877</v>
       </c>
       <c r="F40" t="n">
         <v>1.2419354</v>
@@ -1579,7 +1579,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>1556.9</v>
+        <v>12455.2</v>
       </c>
       <c r="F41" t="n">
         <v>1.59665405</v>
@@ -1607,7 +1607,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>6.18</v>
+        <v>12.36</v>
       </c>
       <c r="F42" t="n">
         <v>0.022</v>
@@ -1631,14 +1631,14 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>06CKA04-1, 06CKA04-1, 4941A04-1, 0604A04-1, 0843A00-1, 4009A04-1, 4009A04-1, 06CKA04-1, 06CKA04-1, 4009A04-1, 4009A04-1</t>
+          <t>06CKA04-1, 4941A04-1, 0604A04-1, 0843A00-1, 4009A04-1, 06CKA04-1, 4009A04-1</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>67.58</v>
+        <v>280.735</v>
       </c>
       <c r="F43" t="n">
-        <v>0.22550861</v>
+        <v>0.129596905</v>
       </c>
     </row>
     <row r="44">
@@ -1663,7 +1663,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>22.66</v>
+        <v>45.32</v>
       </c>
       <c r="F44" t="n">
         <v>0.093184</v>
@@ -1687,14 +1687,14 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>06C9A04-1, 06C9A04-1, 1088A04-1, 1088A04-1, 0604A04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BGA04-1, 06CDA04-1, 0619A04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 01AHA01-1, 01AHA01-1, 01AHA01-1, 06ASA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 1088A04-1, 1088A04-1, 01AHA01-1, 01AHA01-1, 01AHA01-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 01AHA01-1, 01AHA01-1, 01AHA01-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 06C4A04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 06C9A04-1, 06C9A04-1</t>
+          <t>06C9A04-1, 1088A04-1, 0604A04-1, 04BNA04-1, 04BGA04-1, 06CDA04-1, 0619A04-1, 04BNA04-1, 01AHA01-1, 06ASA04-1, 06CEA04-1, 06CEA04-1, 04BNA04-1, 1088A04-1, 01AHA01-1, 06CEA04-1, 01AHA01-1, 04BNA04-1, 06C4A04-1, 04BNA04-1, 06C9A04-1</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>609.755</v>
+        <v>5669.58</v>
       </c>
       <c r="F45" t="n">
-        <v>1.99364141</v>
+        <v>0.95389843</v>
       </c>
     </row>
     <row r="46">
@@ -1715,14 +1715,14 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>0619A04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06ASA04-1, 06ASA04-1, 06ASA04-1, 06ASA04-1, 13A5A03-1, 01BWA03-1, 4017A04-1, 13FTA03-1, 13CBA03-1, 0601A04-1, 04C1A04-1</t>
+          <t>0619A04-1, 06CEA04-1, 06CEA04-1, 06ASA04-1, 06ASA04-1, 13A5A03-1, 01BWA03-1, 4017A04-1, 13FTA03-1, 13CBA03-1, 0601A04-1, 04C1A04-1</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>113.86</v>
+        <v>1148.88</v>
       </c>
       <c r="F46" t="n">
-        <v>0.24139611</v>
+        <v>0.17302811</v>
       </c>
     </row>
     <row r="47">
@@ -1747,7 +1747,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>16.27</v>
+        <v>48.81</v>
       </c>
       <c r="F47" t="n">
         <v>0.022256988</v>
@@ -1775,7 +1775,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>11.29</v>
+        <v>22.58</v>
       </c>
       <c r="F48" t="n">
         <v>0.02494875</v>
@@ -1803,7 +1803,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>30.42</v>
+        <v>91.26000000000001</v>
       </c>
       <c r="F49" t="n">
         <v>0.04847600000000001</v>
@@ -1827,14 +1827,14 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1, 06ASA04-1, 04BNA04-1, 04BNA04-1, 04BNA04-1</t>
+          <t>04BNA04-1, 04BNA04-1, 06ASA04-1, 04BNA04-1</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>24.3</v>
+        <v>48.8</v>
       </c>
       <c r="F50" t="n">
-        <v>0.03087595</v>
+        <v>0.01843065</v>
       </c>
     </row>
     <row r="51">
@@ -1855,14 +1855,14 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>06CEA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1</t>
+          <t>06CEA04-1, 06CEA04-1</t>
         </is>
       </c>
       <c r="E51" t="n">
         <v>59.85000000000001</v>
       </c>
       <c r="F51" t="n">
-        <v>0.2808</v>
+        <v>0.1404</v>
       </c>
     </row>
     <row r="52">
@@ -1887,7 +1887,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>85.11699999999999</v>
+        <v>766.0529999999999</v>
       </c>
       <c r="F52" t="n">
         <v>0.094165765</v>
@@ -1911,14 +1911,14 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>0913B01-1, 01AHA01-1, 01AHA01-1, 06ASA04-1, 06ASA04-1, 06ASA04-1, 06ASA04-1, 0843A00-1, 0924A00-1, 01AHA01-1, 01AHA01-1</t>
+          <t>0913B01-1, 01AHA01-1, 06ASA04-1, 06ASA04-1, 0843A00-1, 0924A00-1, 01AHA01-1</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>97.37</v>
+        <v>379.47</v>
       </c>
       <c r="F53" t="n">
-        <v>0.1293376</v>
+        <v>0.0679448</v>
       </c>
     </row>
     <row r="54">
@@ -1939,14 +1939,14 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>1395A01-1, 06CDA04-1, 06ASA04-1, 06ASA04-1, 06ASA04-1, 06ASA04-1, 3143A08-1, 0843A00-1, 0649A04-1</t>
+          <t>1395A01-1, 06CDA04-1, 06ASA04-1, 06ASA04-1, 3143A08-1, 0843A00-1, 0649A04-1</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>53.49</v>
+        <v>288.33</v>
       </c>
       <c r="F54" t="n">
-        <v>0.09607114999999999</v>
+        <v>0.07165515</v>
       </c>
     </row>
     <row r="55">
@@ -1967,14 +1967,14 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>1395A01-1, 01AHA01-1, 01AHA01-1, 06ASA04-1, 01AHA01-1, 01AHA01-1</t>
+          <t>1395A01-1, 01AHA01-1, 06ASA04-1, 01AHA01-1</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>33.44</v>
+        <v>95.68000000000001</v>
       </c>
       <c r="F55" t="n">
-        <v>0.0436575</v>
+        <v>0.0316975</v>
       </c>
     </row>
     <row r="56">
@@ -2027,7 +2027,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>19.03</v>
+        <v>76.12</v>
       </c>
       <c r="F57" t="n">
         <v>0.0252</v>
@@ -2055,7 +2055,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>25.44</v>
+        <v>127.2</v>
       </c>
       <c r="F58" t="n">
         <v>0.054895</v>
@@ -2079,14 +2079,14 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>04BNA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1</t>
+          <t>04BNA04-1, 06CEA04-1, 06CEA04-1</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>72.34</v>
+        <v>181.11</v>
       </c>
       <c r="F59" t="n">
-        <v>0.1621012</v>
+        <v>0.1059412</v>
       </c>
     </row>
     <row r="60">
@@ -2107,14 +2107,14 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>04BNA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06ASA04-1, 0913B01-1, 0956A00-1, 3143A08-1, 06CEA04-1, 06CEA04-1, 06CEA04-1, 06C6A04-1, 0928A00-1</t>
+          <t>04BNA04-1, 06CEA04-1, 06CEA04-1, 06ASA04-1, 0913B01-1, 0956A00-1, 3143A08-1, 06CEA04-1, 06C6A04-1, 0928A00-1</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>146.25</v>
+        <v>983.7</v>
       </c>
       <c r="F60" t="n">
-        <v>0.44673843</v>
+        <v>0.22209843</v>
       </c>
     </row>
     <row r="61">
@@ -2139,7 +2139,7 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>5.43</v>
+        <v>10.86</v>
       </c>
       <c r="F61" t="n">
         <v>0.0081832</v>
@@ -2163,14 +2163,14 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>06CDA04-1, 06BLA04-1, 06ASA04-1, 06ASA04-1, 06ASA04-1, 06ASA04-1</t>
+          <t>06CDA04-1, 06BLA04-1, 06ASA04-1, 06ASA04-1</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>52.023</v>
+        <v>158.892</v>
       </c>
       <c r="F62" t="n">
-        <v>0.144844</v>
+        <v>0.120428</v>
       </c>
     </row>
     <row r="63">
@@ -2195,7 +2195,7 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>17.8</v>
+        <v>53.40000000000001</v>
       </c>
       <c r="F63" t="n">
         <v>0.041908</v>
@@ -2219,14 +2219,14 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0916A00-1, 0916A00-1, 0916A00-1, 0916A00-1, 0916A00-1, 0916A00-1, 3143A08-1, 04BNA04-1, 0601A04-1, 0619A04-1, 0619A04-1, 0619A04-1, 0619A04-1, 0916A00-1, 0916A00-1, 0916A00-1</t>
+          <t>0916A00-1, 0916A00-1, 3143A08-1, 04BNA04-1, 0601A04-1, 0619A04-1, 0619A04-1, 0916A00-1</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>270.534</v>
+        <v>1436.224</v>
       </c>
       <c r="F64" t="n">
-        <v>0.6506760199999999</v>
+        <v>0.392123634</v>
       </c>
     </row>
     <row r="65">
@@ -2247,14 +2247,14 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>0916A00-1, 0916A00-1, 0944A00-1, 04BNA04-1, 06C6A04-1, 0916A00-1, 0916A00-1, 0154A03-1, 01HJA03-1, 01H8A03-1, 01G4A03-1, 0125A03-1, 1436A01-1, 1306A01-1, 13FDA03-1, 2524A03-1, 2551A03-1</t>
+          <t>0916A00-1, 0944A00-1, 04BNA04-1, 06C6A04-1, 0916A00-1, 0154A03-1, 01HJA03-1, 01H8A03-1, 01G4A03-1, 0125A03-1, 1436A01-1, 1306A01-1, 13FDA03-1, 2524A03-1, 2551A03-1</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>145.915</v>
+        <v>2133.825</v>
       </c>
       <c r="F65" t="n">
-        <v>0.19021034</v>
+        <v>0.1721447</v>
       </c>
     </row>
     <row r="66">
@@ -2275,14 +2275,14 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>0649A04-1, 01AHA01-1, 01AHA01-1, 01AHA01-1, 04BNA04-1, 04BNA04-1, 0928A00-1, 01AHA01-1, 01AHA01-1, 01AHA01-1, 04BNA04-1, 04BNA04-1, 01AHA01-1, 01AHA01-1, 01AHA01-1</t>
+          <t>0649A04-1, 01AHA01-1, 04BNA04-1, 0928A00-1, 01AHA01-1, 04BNA04-1, 01AHA01-1</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>1016.254</v>
+        <v>2681.714</v>
       </c>
       <c r="F66" t="n">
-        <v>1.268184822</v>
+        <v>0.486864886</v>
       </c>
     </row>
     <row r="67">
@@ -2307,7 +2307,7 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>88.459</v>
+        <v>442.295</v>
       </c>
       <c r="F67" t="n">
         <v>0.5059589999999999</v>
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>102.49</v>
+        <v>1127.39</v>
       </c>
       <c r="F68" t="n">
         <v>0.2399201</v>
@@ -2363,7 +2363,7 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>125.775</v>
+        <v>1131.975</v>
       </c>
       <c r="F69" t="n">
         <v>0.1772884</v>
@@ -2391,7 +2391,7 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>10.375</v>
+        <v>20.75</v>
       </c>
       <c r="F70" t="n">
         <v>0.02304975</v>
@@ -2419,7 +2419,7 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>278.274</v>
+        <v>1947.918</v>
       </c>
       <c r="F71" t="n">
         <v>0.37900974</v>
@@ -2447,7 +2447,7 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>16.88</v>
+        <v>50.64000000000001</v>
       </c>
       <c r="F72" t="n">
         <v>0.062337798</v>
@@ -2783,7 +2783,7 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
@@ -2811,7 +2811,7 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>7.51</v>
+        <v>30.04</v>
       </c>
       <c r="F85" t="n">
         <v>0.016485896</v>
@@ -2839,7 +2839,7 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>316.742</v>
+        <v>32941.16800000001</v>
       </c>
       <c r="F86" t="n">
         <v>2.079893602</v>
@@ -2867,7 +2867,7 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>78.627</v>
+        <v>786.27</v>
       </c>
       <c r="F87" t="n">
         <v>0.106812327</v>

</xml_diff>